<commit_message>
Deploying to gh-pages from @ EDGEResearch-CA/TMAtools@4b41eb2fc010cbcda5977c8ea28ba6e09957bb98 🚀
</commit_message>
<xml_diff>
--- a/reference/combined_tma.xlsx
+++ b/reference/combined_tma.xlsx
@@ -342,175 +342,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
+  <dimension ref="C2:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+    <row r="2">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row r="3">
+      <c r="C3" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
+    <row r="7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>13</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>13</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>14</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>14</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+    <row r="8">
+      <c r="C8" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>16</t>
         </is>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ EDGEResearch-CA/TMAtools@2860d502bcef2553af7a85ef82b76af1d7e9b4a0 🚀
</commit_message>
<xml_diff>
--- a/reference/combined_tma.xlsx
+++ b/reference/combined_tma.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="TMA map" sheetId="1" r:id="rId1"/>
     <sheet name="ER" sheetId="2" r:id="rId2"/>
-    <sheet name="TP53" sheetId="3" r:id="rId3"/>
+    <sheet name="P53" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -342,7 +342,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C2:L8"/>
+  <dimension ref="C2:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -361,7 +361,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -369,78 +369,135 @@
           <t>2</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="C3" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>8</t>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>9</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="C7" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -450,69 +507,106 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>11</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>16</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="C8" t="inlineStr">
         <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>11</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>17</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>14</t>
         </is>
       </c>
     </row>
@@ -523,7 +617,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -550,6 +644,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="G1" t="inlineStr">
         <is>
           <t>x</t>
@@ -568,6 +667,11 @@
       <c r="J1" t="inlineStr">
         <is>
           <t>x</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -592,6 +696,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
           <t>0</t>
@@ -608,6 +717,48 @@
         </is>
       </c>
       <c r="J2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>x</t>
         </is>
@@ -634,6 +785,11 @@
           <t>2</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="G6" t="inlineStr">
         <is>
           <t>1</t>
@@ -652,6 +808,11 @@
       <c r="J6" t="inlineStr">
         <is>
           <t>x</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -676,22 +837,49 @@
           <t>9</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
       <c r="I7" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -704,7 +892,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -731,6 +919,11 @@
           <t>8</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
       <c r="G1" t="inlineStr">
         <is>
           <t>5</t>
@@ -747,6 +940,11 @@
         </is>
       </c>
       <c r="J1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
         <is>
           <t>4</t>
         </is>
@@ -773,6 +971,11 @@
           <t>9</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
           <t>3</t>
@@ -791,6 +994,48 @@
       <c r="J2" t="inlineStr">
         <is>
           <t>3</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -815,6 +1060,11 @@
           <t>8</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
       <c r="G6" t="inlineStr">
         <is>
           <t>3</t>
@@ -833,6 +1083,11 @@
       <c r="J6" t="inlineStr">
         <is>
           <t>8</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -857,14 +1112,9 @@
           <t>4</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>9</t>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>5</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -875,6 +1125,38 @@
       <c r="J7" t="inlineStr">
         <is>
           <t>3</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>5</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ EDGEResearch-CA/TMAtools@2b758d622b101a0a55cc544f1b0708c81b2df8b8 🚀
</commit_message>
<xml_diff>
--- a/reference/combined_tma.xlsx
+++ b/reference/combined_tma.xlsx
@@ -8,8 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="TMA map" sheetId="1" r:id="rId1"/>
-    <sheet name="ER" sheetId="2" r:id="rId2"/>
-    <sheet name="P53" sheetId="3" r:id="rId3"/>
+    <sheet name="er" sheetId="2" r:id="rId2"/>
+    <sheet name="p53" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ EDGEResearch-CA/TMAtools@cc512a52320f5aa41474319da765f7c5587d56bd 🚀
</commit_message>
<xml_diff>
--- a/reference/combined_tma.xlsx
+++ b/reference/combined_tma.xlsx
@@ -617,269 +617,269 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K8"/>
+  <dimension ref="C2:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>x</t>
+          <t>9</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -892,269 +892,269 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K8"/>
+  <dimension ref="C2:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+    <row r="2">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row r="3">
+      <c r="C3" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+    <row r="4">
+      <c r="C4" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="M7" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+    <row r="8">
+      <c r="C8" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>5</t>
         </is>

</xml_diff>